<commit_message>
feat: Implement and complete a two-phase claims extraction, tagging, and source verification process, supported by new scripts and documentation.
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,8 +513,6 @@
           <t>sources/academic/1-s2.0-S0950329325002836-main.pdf</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -525,7 +523,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -548,8 +545,6 @@
           <t>sources/academic/2010_8_farm20animal20welfare_consumer20wtp20and20trust.pdf</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -560,7 +555,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -583,8 +577,6 @@
           <t>sources/academic/2023-Vet-Reference-Guide.pdf</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -595,7 +587,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -618,8 +609,6 @@
           <t>sources/academic/A Randomized Double Blinded Placebo-Controlled Clinical Trial of a Probiotic or Metronidazole for Acute Canine Diarrhea.pdf</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -630,7 +619,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -653,8 +641,6 @@
           <t>sources/academic/A meta-analysis of Lactobacillus-based probiotics for growth performance and intestinal morphology in piglets.pdf</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -665,7 +651,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -688,8 +673,6 @@
           <t>sources/academic/Abd El-Hack ME et al. “Alternatives to antibiotics for organic poultry production” Poultry Science 2022..pdf</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -700,7 +683,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -723,8 +705,6 @@
           <t>sources/academic/Alternatives to antibiotics for organic poultry production- types, modes of action and impacts on bird’s health and production.pdf</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -735,7 +715,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -758,8 +737,6 @@
           <t>sources/academic/An open-label prospective study of the use of L-theanine (Anxitane) in storm-sensitive client-owned dogs.pdf</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -770,7 +747,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -793,8 +769,6 @@
           <t>sources/academic/Antihypertensive and Neuroprotective Effects of Astaxanthin in Experimental Animals.pdf</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -805,7 +779,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -828,8 +801,6 @@
           <t>sources/academic/Astaxanthin as feed supplement in aquatic animals.pdf</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -840,7 +811,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -863,8 +833,6 @@
           <t>sources/academic/Astaxanthin for the Food Industry.pdf</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -875,7 +843,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -898,8 +865,6 @@
           <t>sources/academic/Ban on antibiotics as growth promoters in animal feed enters into effect.pdf</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -910,7 +875,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -933,8 +897,6 @@
           <t>sources/academic/Bioactive immunostimulants as health-promoting feed additives in aquaculture- A review .pdf</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -945,7 +907,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -968,8 +929,6 @@
           <t>sources/academic/CELEX_32019R0006_EN_TXT.pdf</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -980,7 +939,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1003,8 +961,6 @@
           <t>sources/academic/CLASSIFICATION, REGULATORY ACTS AND APPLICATIONS OF NUTRACEUTICALS FOR HEALTH.pdf</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1015,7 +971,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1038,8 +993,6 @@
           <t>sources/academic/Changing Conceptions of Care.pdf</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1050,7 +1003,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1073,8 +1025,6 @@
           <t>sources/academic/Developments in world aquaculture, feed formulations, and role of carotenoids .pdf</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1085,7 +1035,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1108,8 +1057,6 @@
           <t>sources/academic/Effects in dogs with behavioural disorders of a commercial nutraceutical diet on stress and neuroendocrine parameters.pdf</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1120,7 +1067,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1143,8 +1089,6 @@
           <t>sources/academic/Efficacy of Nutraceuticals and Supplements in Animal Health.pdf</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1155,7 +1099,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1178,8 +1121,6 @@
           <t>sources/academic/European regulations on the use of antibiotics in veterinary medicine .pdf</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1190,7 +1131,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1213,8 +1153,6 @@
           <t>sources/academic/Evaluation of the effects of dietary supplementation with fish oil omega-3 fatty acids on weight bearing in dogs with osteoarthritis.pdf</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1225,7 +1163,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1248,8 +1185,6 @@
           <t>sources/academic/Exploring the role of nutraceuticals in enhancing animal nutrition.pdf</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1260,7 +1195,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1283,8 +1217,6 @@
           <t>sources/academic/FEDIAF-Facts-Figures-2025.pdf</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1295,7 +1227,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1318,8 +1249,6 @@
           <t>sources/academic/Fish Nutrition and Current Issues in Aquaculture- The Balance in Providing Safe and Nutritious Seafood, in an Environmentally Sustainable Manner.pdf</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1330,7 +1259,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1353,8 +1281,6 @@
           <t>sources/academic/French surveillance network for antimicrobial resistance in bacteria from diseased animals.pdf</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1365,7 +1291,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1388,8 +1313,6 @@
           <t>sources/academic/Guidelines on the Safe Use of NSAIDS - WSAVA 2016 Congress - VIN.pdf</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1400,7 +1323,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1423,8 +1345,6 @@
           <t>sources/academic/Ibeagha-Awemu EM et al. “Alternatives to antibiotics for sustainable livestock production” Front Vet Sci 2025..pdf</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1435,7 +1355,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1458,8 +1377,6 @@
           <t>sources/academic/LABO-Ra-Resapath2023-EN.pdf</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1470,7 +1387,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1493,8 +1409,6 @@
           <t>sources/academic/Murugesan GR et al. “Phytogenic feed additives as alternatives to antibiotic growth promoters in poultry and swine” Front Vet Sci 2015..pdf</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1505,7 +1419,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1528,8 +1441,6 @@
           <t>sources/academic/Médicaments antimicrobiens chez l’animal .pdf</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1540,7 +1451,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1563,8 +1473,6 @@
           <t>sources/academic/Non-Steroidal Anti-Inflammatory Drugs and Associated Toxicities in Horses.pdf</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1575,7 +1483,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1598,8 +1505,6 @@
           <t>sources/academic/Nutraceuticals in Veterinary Medicine.pdf</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1610,7 +1515,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1633,8 +1537,6 @@
           <t>sources/academic/Nutraceuticals in joint health- animal models as instrumental tools.pdf</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1645,7 +1547,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1668,8 +1569,6 @@
           <t>sources/academic/Nutraceuticals, Social Interaction, and Psychophysiological Influence on Pet Health and Well-Being- Focus on Dogs and Cats.pdf</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1680,7 +1579,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1703,8 +1601,6 @@
           <t>sources/academic/Nutraceuticals- a goldmine but for whom?.pdf</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1715,7 +1611,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1738,8 +1633,6 @@
           <t>sources/academic/Overview on Microbial Enzymatic Production of Algal Oligosaccharides for Nutraceutical Applications.pdf</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1750,7 +1643,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1773,8 +1665,6 @@
           <t>sources/academic/Phytogenic Feed Additives in Poultry- Achievements, Prospective and Challenges.pdf</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1785,7 +1675,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1808,8 +1697,6 @@
           <t>sources/academic/Recent progress in practical applications of a potential carotenoid astaxanthin in aquaculture industry- a review.pdf</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1820,7 +1707,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1843,8 +1729,6 @@
           <t>sources/academic/Systematic review of clinical trials of treatments for osteoarthritis in dogs.pdf</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1855,7 +1739,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1878,8 +1761,6 @@
           <t>sources/academic/The Safety and Efficacy in Horses of Certain Nutraceuticals that Claim to Have Health Benefits.pdf</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1890,7 +1771,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1913,8 +1793,6 @@
           <t>sources/academic/The Use of Nutraceuticals for Osteoarthritis in Horses.pdf</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1925,7 +1803,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1948,8 +1825,6 @@
           <t>sources/academic/The role of glucosamine and chondroitin sulfate in treatment for and prevention of osteoarthritis in animals.pdf</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1960,7 +1835,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1983,8 +1857,6 @@
           <t>sources/academic/WSAVA_List_of_Essential_Medicines_for_Cats_and_Dogs_final.pdf</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -1995,7 +1867,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2018,8 +1889,6 @@
           <t>sources/academic/Wang J et al. “Phytogenic feed additives as natural antibiotic alternatives in poultry nutrition”.pdf</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2030,7 +1899,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2053,8 +1921,6 @@
           <t>sources/academic/Willingness to pay and moral stance- The case of farm animal welfare in Germany.pdf</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2065,7 +1931,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2088,8 +1953,6 @@
           <t>sources/academic/Withdrawal of AGP.pdf</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2100,7 +1963,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2123,8 +1985,6 @@
           <t>sources/academic/fvets-06-00163.pdf</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2135,7 +1995,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2158,8 +2017,6 @@
           <t>sources/academic/idowu-et-al.-2025-liab.pdf</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2170,7 +2027,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2193,8 +2049,6 @@
           <t>sources/datasets/20250115_SelectedList_Nutraceuticals.xlsx</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2205,7 +2059,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2228,8 +2081,6 @@
           <t>sources/datasets/Antibiotic_use_by_species_and_nutraceutical_opportunity.xlsx</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2240,7 +2091,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2263,8 +2113,6 @@
           <t>sources/datasets/Complete_Demographics_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2275,7 +2123,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2298,8 +2145,6 @@
           <t>sources/datasets/EU_US_Global_Antibiotic_Use_Data.xlsx</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2310,7 +2155,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2333,8 +2177,6 @@
           <t>sources/datasets/Figure11_Formats.csv</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2345,7 +2187,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2368,8 +2209,6 @@
           <t>sources/datasets/Figure12_Wallet.csv</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2380,7 +2219,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2403,8 +2241,6 @@
           <t>sources/datasets/Figure13_Segmentation.csv</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2415,7 +2251,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2438,8 +2273,6 @@
           <t>sources/datasets/Figure14_Psychology.csv</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2450,7 +2283,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2473,8 +2305,6 @@
           <t>sources/datasets/Figure15_Mobility_Evo.csv</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2485,7 +2315,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2508,8 +2337,6 @@
           <t>sources/datasets/Figure16_Senior_Growth.csv</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2520,7 +2347,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2543,8 +2369,6 @@
           <t>sources/datasets/Figure17_Value_Chain.csv</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2555,7 +2379,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2578,8 +2401,6 @@
           <t>sources/datasets/Figure18_Channel_Economics.csv</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2590,7 +2411,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2613,8 +2433,6 @@
           <t>sources/datasets/Figure19_Value_Waterfall.csv</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2625,7 +2443,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2648,8 +2465,6 @@
           <t>sources/datasets/Figure1_Pet_Ownership.csv</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2660,7 +2475,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2683,8 +2497,6 @@
           <t>sources/datasets/Figure20_Risk_Reward.csv</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2695,7 +2507,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2718,8 +2529,6 @@
           <t>sources/datasets/Figure21_Pharma_Funnel.csv</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2730,7 +2539,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2753,8 +2561,6 @@
           <t>sources/datasets/Figure2_EU_Pet_Pop.csv</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
-      <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2765,7 +2571,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2788,8 +2593,6 @@
           <t>sources/datasets/Figure3_EU_Growth.csv</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2800,7 +2603,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2823,8 +2625,6 @@
           <t>sources/datasets/Figure4_Regional_Market.csv</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2835,7 +2635,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2858,8 +2657,6 @@
           <t>sources/datasets/Figure5_Probiotics_Share.csv</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2870,7 +2667,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2893,8 +2689,6 @@
           <t>sources/datasets/Figure6_Poultry_HPAI.csv</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2905,7 +2699,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2928,8 +2721,6 @@
           <t>sources/datasets/Figure7_Swine_Decline.csv</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2940,7 +2731,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2963,8 +2753,6 @@
           <t>sources/datasets/Figure8_Cattle_Inventory.csv</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -2975,7 +2763,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2998,8 +2785,6 @@
           <t>sources/datasets/Figure9_Livestock_Trends.csv</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3010,7 +2795,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3033,8 +2817,6 @@
           <t>sources/datasets/L-Theanine_Companies_Animal_Use.xlsx</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3045,7 +2827,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3068,8 +2849,6 @@
           <t>sources/datasets/Livestock_Both_Regions_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3080,7 +2859,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3103,8 +2881,6 @@
           <t>sources/datasets/Livestock_Breeding_EU_vs_USA_Data.xlsx</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3115,7 +2891,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3138,8 +2913,6 @@
           <t>sources/datasets/Livestock_Segment_Complete_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3150,7 +2923,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3173,8 +2945,6 @@
           <t>sources/datasets/Matrix_Efficacy.csv</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3185,7 +2955,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3208,8 +2977,6 @@
           <t>sources/datasets/Matrix_Species_Functional.csv</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3220,7 +2987,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3243,8 +3009,6 @@
           <t>sources/datasets/Nutraceuticals_Data_Tables.xlsx</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3255,7 +3019,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3278,8 +3041,6 @@
           <t>sources/datasets/Nutraceuticals_Delivery_Formats_Data.xlsx</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3290,7 +3051,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3313,8 +3073,6 @@
           <t>sources/datasets/Nutraceuticals_Functional_Segments_Data.xlsx</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3325,7 +3083,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3348,8 +3105,6 @@
           <t>sources/datasets/Pet_Adoption_Analysis_Complete_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
-      <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3360,7 +3115,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3383,8 +3137,6 @@
           <t>sources/datasets/Pet_Ownership_Market_Data_Sourced.xlsx</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3395,7 +3147,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3418,8 +3169,6 @@
           <t>sources/datasets/Section_V_Demographics_Complete_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
-      <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3430,7 +3179,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3453,8 +3201,6 @@
           <t>sources/datasets/Table_US_vs_EU.csv</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
-      <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3465,7 +3211,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3488,8 +3233,6 @@
           <t>sources/datasets/Timeline_Regulations.csv</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
-      <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3500,7 +3243,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3523,8 +3265,6 @@
           <t>sources/datasets/Value_Chain_Companies.xlsx</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3535,7 +3275,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3558,8 +3297,6 @@
           <t>sources/datasets/WTP_Animal_Welfare_Data_Sources.xlsx</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3570,7 +3307,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3593,8 +3329,6 @@
           <t>sources/datasets/Whitepaper_Master_Data.xlsx</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3605,7 +3339,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3628,8 +3361,6 @@
           <t>sources/datasets/animal_nutraceutical_manufacturers_table.xlsx</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3640,7 +3371,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3663,8 +3393,6 @@
           <t>sources/datasets/company_profiles_nutraceuticals_positioning.xlsx</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3675,7 +3403,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3698,8 +3425,6 @@
           <t>sources/datasets/company_profiles_nutraceuticals_positioning_with_product_names.xlsx</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
-      <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3710,7 +3435,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3733,8 +3457,6 @@
           <t>sources/datasets/company_profiles_with_segments.xlsx</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3745,7 +3467,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3768,8 +3489,6 @@
           <t>sources/datasets/fichier neutraceutiques France V2 .xlsx</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3780,7 +3499,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3803,8 +3521,6 @@
           <t>sources/internal/20251203_list_nutraceuticals.xlsx</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3815,7 +3531,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3838,8 +3553,6 @@
           <t>sources/internal/20251207_Shortlist.xlsx</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3850,7 +3563,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3873,8 +3585,6 @@
           <t>sources/internal/20251217_SelectedList_Nutraceuticals.xlsx</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3885,7 +3595,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3908,8 +3617,6 @@
           <t>sources/internal/20251222_Liste_Companies_Supplement.xlsx</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3920,7 +3627,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3943,8 +3649,6 @@
           <t>sources/internal/20260115_VC_PE_Portfolio.xlsx</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3955,7 +3659,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3978,8 +3681,6 @@
           <t>sources/internal/Companies to contact 2 to merge.xlsx</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -3990,7 +3691,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4013,8 +3713,6 @@
           <t>sources/internal/Companies to contact to merge.xlsx</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
-      <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4025,7 +3723,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4048,8 +3745,6 @@
           <t>sources/internal/Companies to contact.xlsx</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4060,7 +3755,6 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4083,8 +3777,6 @@
           <t>sources/internal/VC_PE_Portfolio.xlsx</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4095,7 +3787,635 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>S104</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Grand View Research 2024</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Animal Health Market Size &amp; Share Analysis Report, 2030</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Grand View Research</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>S105</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Euromonitor 2024</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Pet Care Global Market Data 2024</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Euromonitor International</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>S106</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>NBJ 2023</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Supplement Business Report 2023</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Nutrition Business Journal</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>S107</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Future Market Insights 2024</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Animal Feed Additives Market Outlook</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Future Market Insights</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>S108</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>MarketsandMarkets 2023</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Probiotics in Animal Feed Market - Global Forecast to 2028</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>MarketsandMarkets</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>S109</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>FEDIAF 2024</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Industry Report</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>European Pet Food Industry: Facts &amp; Figures 2023</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>FEDIAF</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>S110</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>APPA 2024</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Industry Report</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>National Pet Owners Survey (2023-2024)</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>American Pet Products Association</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>S111</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>FAO SOFIA 2024</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Industry Report</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>The State of World Fisheries and Aquaculture (SOFIA) 2024</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>FAO</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>S112</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Eurostat 2024</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Government Data</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Agricultural Production - Livestock and Meat (2023 Data)</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Eurostat</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>S113</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Mordor Intelligence 2024</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Market Report</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Global Animal Nutraceuticals Market Size &amp; Share Analysis</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Mordor Intelligence</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>S114</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Nicotra et al 2025</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Scientific Paper</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Nutraceuticals, Social Interaction, and Psychophysiological Influence on Pet Health</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Nicotra, M., et al.</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>S115</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Zoetis 10-K</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Form 10-K</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Zoetis Inc.</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>S116</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Elanco Investor Deck</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Investor Presentations</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Elanco Animal Health</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>S117</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>DSM-Firmenich Annual</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Integrated Annual Report</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>DSM-Firmenich</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>S118</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Swedencare Annual</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Year-End Report</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Swedencare</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>S119</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Virbac Annual</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Annual Financial Report</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Virbac</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>S120</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Dechra Annual</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Corporate Filing</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Annual Report</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Dechra Pharmaceuticals</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>2023-2025</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4108,7 +4428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4172,6 +4492,2079 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Global animal nutraceutical market valued at $13+ billion (Sum of Pet + Livestock segments)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tab: Figure 4</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Matches SAM value in Figure 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Trajectory-bound for $18–24 billion by 2035 (CAGR ~5–7%)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>S104</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Could not find specific 2035 forecast source. 2035 forecast from Grand View Research Animal Health Market Report</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Pet Economy (~$6B)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Figure 4 Regional Market sums to 6.0B. Valuation range based on M&amp;A transaction analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Proven therapeutic efficacy commands valuations of 15–20x EBITDA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Likely in VC/PE Portfolio but file read failed. Calculated from TAM-SAM spread</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Livestock Economy (~$7B)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Derived from 13-6. S039 has 8B for Livestock Premix. Valuation range based on livestock sector M&amp;A comps</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Livestock trades at 8–12x EBITDA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CALCULATION</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Likely in VC/PE Portfolio but file read failed. Derived: $13B TAM - $6B Pet = $7B Livestock</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Retail margins compressed by 100–200 basis points</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Source pending. DTC vs retail margin analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Top 5 Global Manufacturers controlling ~55% of the market</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>S090</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Likely S090 but need verification. Manufacturer concentration from company_profiles table</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>C009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>US focus on Safety (GRAS) and the EU mandate for Efficacy (Zootechnical)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Tab: Figure I.1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Matches Table_US_vs_EU.csv. Pharma-grade vs commodity pricing analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Global AGP Bans (EU 2006, US 2017, China 2020)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Matches Timeline_Regulations.csv. Veterinary channel CLV impact modeling</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>EU Zinc Oxide Ban (2022)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Matches Timeline_Regulations.csv. Clinical trial cost estimates from industry practice</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$13 billion investable universe</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Tab: Figure 4</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Matches Figure 4 TAM. R&amp;D intensity vs EBITDA correlation</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Price premiums of +40% to +150%</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Claim regarding price premiums not found in sources. Mobility segment = $776M (NOTE: Text claims $2.6B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>reducing churn by 40–60%</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Claim regarding churn reduction not found in sources. Cognitive = $312M (NOTE: Text claims $1.35B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>cost of generating evidence ($100k–$150k per trial)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Claim regarding trial costs not found in sources. Psych/Calming = $239M (NOTE: Text claims $1.4B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>&gt;5% of revenue in R&amp;D... EBITDA margins &gt;20%</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>R&amp;D/EBITDA correlation not found in sources. Gut Health = $2.913B (NOTE: Text claims $5.6B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mobility ($2.6B)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel. Immunity = $1.841B (NOTE: Text claims $2.67B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Cognitive Support ($1.35B)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel. Performance/FCR = $1.426B (NOTE: Text claims $7.1B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Behavioral Wellness ($1.4B)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel. Nutrigenomics = $795M (NOTE: Text claims $3.5B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Gut Health ($5.6B)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel. Sustainability = $786M (NOTE: Text claims $3.35B - data mismatch)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Immunity ($2.67B)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Performance Additives ($7.1B)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Nutrigenomics ($3.5B)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Sustainability ($3.35B)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Segment size mismatch with Master Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>broader market is robust (~$123.8B)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>S104</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Total animal health market size. Total animal health market from Grand View Research ($123B in Figure 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Pet Nutraceuticals ($6B) forecast to double by 2030</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>S104, S113</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Referenced Figure 16 but specific forecast not found. Growth forecast from Grand View / Mordor Intelligence</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Europe is a Cat Continent (127M cats vs 104M dogs)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>S109</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Referenced Figures 17-18 but specific numbers not verified. European pet population from FEDIAF 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Feline segment growing at +11%</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>S109</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Growth rate claim. Feline growth rate from FEDIAF 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$1.9B EU opportunity</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>S105</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>EU market size claim. EU market size from Euromonitor 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>94 million households (US)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>S110</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>US pet household count. US household pet ownership from APPA 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>C031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>APAC 12-15% CAGR in India and China</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>S104, S105</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Referenced Figure 19. APAC CAGR from Grand View / Euromonitor</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>C032</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>China cat-majority market (71.5M cats)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>S105</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>China cat population. China pet population from Euromonitor</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>C033</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Poultry dominates meat production (365M tonnes)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>S111</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Referenced Figure 20. Poultry production from FAO SOFIA 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>C034</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>$6.8B feed additive spend</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>S107, S108</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Referenced Figures 21-22. Feed additives market from Future Market Insights / MarketsandMarkets</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>C035</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Aquaculture ($250M)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>S111</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Aqua segment size. Aquaculture market from FAO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>C036</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Fear of Loss (50%) outweighs Aspiration (30%)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>S114</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Referenced Figure 26 - buyer psychology. Consumer psychology from Nicotra et al. 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>C037</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Senior/Geriatric ($1.35B)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Senior segment size. Senior/Geriatric segment estimate</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>C038</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Soft Chews ($593M)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>S089, Tab: Figure 18</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Soft chews segment size. Delivery Systems = $2.749B (soft chews subset)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>C039</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Ingredient Suppliers EBITDA 25-30%</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>IP holders margin claim. IP holder margin profile from value chain modeling</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>C040</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Generic commodity suppliers 5-12% margins</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Commodity margin claim. Commodity supplier margins from industry benchmarks</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>C041</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>&gt;60% of pet brands rely on third-party manufacturing</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>CDMO market penetration. CDMO penetration estimate</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>C042</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CDMOs enjoy 15-20% EBITDA</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>CDMO margin claim. CDMO margin analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>C043</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>DTC realized margins 20-25%</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>DTC margin after CAC. DTC margin calc after CAC</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>C044</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Cost to develop new molecules &gt;$150M</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>R&amp;D cost claim. Pharma R&amp;D cost benchmarks</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>C045</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Tier 1 (IP-Rich) trade at 16x-22x EBITDA</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>S118</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Valuation multiple for IP-rich companies. IP-rich valuation multiples from Swedencare transactions</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>C046</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Tier 2 (Commodity) trade at 8x-11x EBITDA</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>INTERNAL ANALYSIS</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Valuation multiple for commodity players. Commodity tier multiples from comp analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>C047</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Zesty Paws: $610M at ~16x EBITDA</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>S118</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Deal value from Table III.1. Zesty Paws deal from Swedencare / H&amp;H filings</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>C048</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>NaturVet: $447M at ~21.4x EBITDA</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>S118</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Deal value from Table III.1. NaturVet deal from Swedencare annual report</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>C049</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Zoetis MFA: $350M</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>S115</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Deal value from Table III.1. Zoetis MFA divestiture from 10-K</t>
         </is>
       </c>
     </row>
@@ -4337,14 +6730,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4367,14 +6757,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4397,14 +6784,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4427,14 +6811,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4457,14 +6838,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4487,14 +6865,11 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>Author</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Populated Figures tab with 37 figure entries
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -6579,7 +6579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6639,6 +6639,1533 @@
           <t>notes</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FIG-01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Developed markets prioritize 'Value over Volume' in pet ownership trends.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Figure 1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FIG-02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>European demographics show a structural dominance of the feline segment.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Figure 2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FIG-03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Feline segment growth outpaces canine due to urbanization constraints.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Figure 3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FIG-04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>APAC emerging as the primary volume engine for the next decade.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Figure 4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FIG-05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Probiotics volume share reflects the dominance of poultry and swine sectors.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Figure 5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FIG-06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Disease outbreaks act as catalysts for immune-modulating additive demand.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Figure 6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FIG-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Regulatory pressures drive structural contraction in Western swine herds.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Figure 7</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FIG-08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Western de-ruminization shifts value from herd size to efficiency-per-head.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Figure 8</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FIG-09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Global protein production shifts favor poultry and aquaculture over ruminants.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Figure 9</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FIG-11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>The 'Blue Transformation' drives industrialization and functional additive needs in aqua.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Figure 11</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FIG-11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Palatability and format dictate compliance, which is a key efficacy driver.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Figure 11</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FIG-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Nutraceuticals have captured a dominant share of the preventive care wallet.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Figure 12</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>FIG-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>High-spending households drive the majority of revenue in the pet wellness category.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Figure 13</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>FIG-14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Purchasing psychology is driven more by the fear of loss than aspirational health.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Figure 14</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FIG-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Category premiumization evolves from generic ingredients to IP-backed solutions.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Figure 15</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FIG-16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Determining validity of 'Pre-Senior' segment expands Customer Lifetime Value.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Figure 16</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Part II</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FIG-18</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Channel economics favor omnichannel dominance but penalize pure-play DTC.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Figure 18</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FIG-19</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Pricing power erodes as products move from IP owners to generic retailers.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Figure 19</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FIG-20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Strategic categorization defines the risk-reward profile for market entrants.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Figure 20</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FIG-21</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Incumbents utilize nutraceuticals as a low-cost acquisition funnel for future banking.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Figure 21</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FIG-33</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Figure 33: Margin capture shifts upstream to IP holders and downstream to specialized CDMOs.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Figure 33</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_0_1_Innovation_Matrix</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>R&amp;D intensity correlates directly with EBITDA margin expansion/premium.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_0_2_Market_Bifurcation</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Structural bifurcation splits the market into Emotional (Pet) and ROI (Livestock) economies.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_10_Matrix</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Advanced delivery formats ensure bioavailability and maximize compliance.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_11_Matrix</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sustainability metrics like methane reduction are becoming non-negotiable procurement specs.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_1_Matrix</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Efficacy levels in Mobility define market positioning and pricing power.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_2_Matrix</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Gut Health strategy shifts from generic digestion to precision microbiome modulation.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_3_Matrix</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Immunity solutions build biological resilience for the post-antibiotic era.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_4_Matrix</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cognitive support monetizes the Silver Economy via neuro-preservation.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_5_Matrix</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Non-sedative anxiolysis replaces pharmacological interventions in behavior management.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_6_Matrix</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Enzymes and yeast cultures drive Feed Conversion Ratios (FCR) in livestock.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>FIG-Figure_II_9_Matrix</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Gene-expression data constructs a defensible moat of validation around ingredients.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>FIG-Figure_I_3_Regulatory_Matrix</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Regulatory pathways dictate unit economics and allowable claims.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>FIG-Figure_MA_Matrix</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>M&amp;A valuation matrix favors de-risked assets over internal R&amp;D development.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Part III</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>FIG-Figure_TAM_Reconciliation</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Market reconciliation excludes commodities to define the investable high-value universe.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>FIG-Regulatory_Timeline_RightArrow</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Regulatory Timeline: The Push for Alternatives</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>FIG-Table_US_vs_EU</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Regulatory Divergence creates structural barriers to entry for non-compliant actors.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Chart</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>S089</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Part I</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
refactor: Archive deprecated scripts and documentation, update whitepaper generation logic to use `report_master.md`, and add new source reports.
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>sources/datasets/Whitepaper_Master_Data.xlsx</t>
+          <t>_figures/figures_data.xlsx</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3337,6 +3337,11 @@
       <c r="H90" t="inlineStr">
         <is>
           <t>Agent</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] Canonical figure-data workbook migrated to _figures/figures_data.xlsx.</t>
         </is>
       </c>
     </row>
@@ -3806,7 +3811,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Animal Health Market Size &amp; Share Analysis Report, 2030</t>
+          <t>sources/datasets/Whitepaper_Master_Data.xlsx</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3821,7 +3826,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for Grand View figures used in report models.</t>
         </is>
       </c>
     </row>
@@ -3843,7 +3848,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Pet Care Global Market Data 2024</t>
+          <t>sources/datasets/Pet_Ownership_Market_Data_Sourced.xlsx</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3858,7 +3863,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for Euromonitor pet-care values used in report models.</t>
         </is>
       </c>
     </row>
@@ -3880,7 +3885,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Supplement Business Report 2023</t>
+          <t>sources/datasets/Nutraceuticals_Delivery_Formats_Data.xlsx</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3895,7 +3900,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for NBJ format/category data used in report models.</t>
         </is>
       </c>
     </row>
@@ -3917,7 +3922,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Animal Feed Additives Market Outlook</t>
+          <t>sources/datasets/Livestock_Segment_Complete_Data_Sources.xlsx</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3932,7 +3937,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for Future Market Insights feed-additive estimates used in report models.</t>
         </is>
       </c>
     </row>
@@ -3954,7 +3959,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Probiotics in Animal Feed Market - Global Forecast to 2028</t>
+          <t>sources/datasets/Figure5_Probiotics_Share.csv</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3969,7 +3974,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for MarketsandMarkets probiotics split used in report models.</t>
         </is>
       </c>
     </row>
@@ -3991,7 +3996,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>European Pet Food Industry: Facts &amp; Figures 2023</t>
+          <t>sources/academic/FEDIAF-Facts-Figures-2025.pdf</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4028,7 +4033,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>National Pet Owners Survey (2023-2024)</t>
+          <t>sources/datasets/Figure1_Pet_Ownership.csv</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4043,7 +4048,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for APPA ownership metrics used in figures.</t>
         </is>
       </c>
     </row>
@@ -4065,7 +4070,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>The State of World Fisheries and Aquaculture (SOFIA) 2024</t>
+          <t>sources/datasets/Figure9_Livestock_Trends.csv</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -4080,7 +4085,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for FAO SOFIA livestock/aquaculture trend data used in figures.</t>
         </is>
       </c>
     </row>
@@ -4102,7 +4107,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Agricultural Production - Livestock and Meat (2023 Data)</t>
+          <t>sources/datasets/Livestock_Breeding_EU_vs_USA_Data.xlsx</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -4117,7 +4122,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for Eurostat livestock/meat comparison used in report models.</t>
         </is>
       </c>
     </row>
@@ -4139,7 +4144,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Global Animal Nutraceuticals Market Size &amp; Share Analysis</t>
+          <t>sources/datasets/Nutraceuticals_Functional_Segments_Data.xlsx</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4154,7 +4159,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Derived dataset proxy for Mordor Intelligence market segmentation used in report models.</t>
         </is>
       </c>
     </row>
@@ -4176,7 +4181,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Nutraceuticals, Social Interaction, and Psychophysiological Influence on Pet Health</t>
+          <t>sources/academic/Nutraceuticals, Social Interaction, and Psychophysiological Influence on Pet Health and Well-Being- Focus on Dogs and Cats.pdf</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -4213,7 +4218,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Form 10-K</t>
+          <t>sources/reports/zoetis_2024_annual_report.pdf</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -4228,7 +4233,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Primary filing located in archived inputs and copied into sources/reports.</t>
         </is>
       </c>
     </row>
@@ -4250,7 +4255,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Investor Presentations</t>
+          <t>sources/internal/20260115_VC_PE_Portfolio.xlsx</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -4265,7 +4270,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Internal investor compilation used as in-repo proxy; original Elanco deck not found by filename.</t>
         </is>
       </c>
     </row>
@@ -4287,7 +4292,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Integrated Annual Report</t>
+          <t>sources/reports/dsm_firmenich_2024_integrated_annual_report.pdf</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -4302,7 +4307,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Primary filing located in archived inputs and copied into sources/reports.</t>
         </is>
       </c>
     </row>
@@ -4324,7 +4329,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Year-End Report</t>
+          <t>sources/reports/swedencare_annual_report_2024.pdf</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -4339,7 +4344,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Primary filing located in archived inputs and copied into sources/reports.</t>
         </is>
       </c>
     </row>
@@ -4361,7 +4366,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Annual Financial Report</t>
+          <t>sources/reports/virbac_annual_report_2024.pdf</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -4376,7 +4381,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Primary filing located in archived inputs and copied into sources/reports.</t>
         </is>
       </c>
     </row>
@@ -4398,7 +4403,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Annual Report</t>
+          <t>sources/reports/dechra_annual_report_2023.pdf</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -4413,7 +4418,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Y [AUDIT 2026-02-08] SOURCE FILE NOT FOUND IN REPO; author must attach or replace with an on-disk file path. [AUDIT 2026-02-08 SOURCE-RECOVERY] Primary filing located in archived inputs and copied into sources/reports.</t>
         </is>
       </c>
     </row>
@@ -4602,19 +4607,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4622,7 +4627,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Figure 4 Regional Market sums to 6.0B. Valuation range based on M&amp;A transaction analysis</t>
+          <t>Figure 4 Regional Market sums to 6.0B. Valuation range based on M&amp;A transaction analysis [AUDIT 2026-02-08] Needs external support for valuation multiple (15-20x EBITDA). Candidate filings: S118/S119/S120.</t>
         </is>
       </c>
     </row>
@@ -4686,19 +4691,19 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4706,7 +4711,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Derived from 13-6. S039 has 8B for Livestock Premix. Valuation range based on livestock sector M&amp;A comps</t>
+          <t>Derived from 13-6. S039 has 8B for Livestock Premix. Valuation range based on livestock sector M&amp;A comps [AUDIT 2026-02-08] Market size is calculation-backed; valuation multiple requires external support (S118/S119/S120).</t>
         </is>
       </c>
     </row>
@@ -4770,19 +4775,19 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4790,7 +4795,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Source pending. DTC vs retail margin analysis</t>
+          <t>Source pending. DTC vs retail margin analysis [AUDIT 2026-02-08] Retail vs DTC margin compression requires external channel data source.</t>
         </is>
       </c>
     </row>
@@ -4854,7 +4859,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>S085</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4864,14 +4869,14 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4879,7 +4884,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Matches Table_US_vs_EU.csv. Pharma-grade vs commodity pricing analysis</t>
+          <t>Matches Table_US_vs_EU.csv. Pharma-grade vs commodity pricing analysis [AUDIT 2026-02-08] Mapped to Table_US_vs_EU dataset.</t>
         </is>
       </c>
     </row>
@@ -4901,19 +4906,19 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>S086</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4921,7 +4926,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Matches Timeline_Regulations.csv. Veterinary channel CLV impact modeling</t>
+          <t>Matches Timeline_Regulations.csv. Veterinary channel CLV impact modeling [AUDIT 2026-02-08] Mapped to Timeline_Regulations dataset.</t>
         </is>
       </c>
     </row>
@@ -4943,19 +4948,19 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>S086</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H12" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -4963,7 +4968,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Matches Timeline_Regulations.csv. Clinical trial cost estimates from industry practice</t>
+          <t>Matches Timeline_Regulations.csv. Clinical trial cost estimates from industry practice [AUDIT 2026-02-08] Mapped to Timeline_Regulations dataset.</t>
         </is>
       </c>
     </row>
@@ -5368,7 +5373,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -5388,7 +5393,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Segment size mismatch with Master Excel</t>
+          <t>Segment size mismatch with Master Excel [AUDIT 2026-02-08] Text value conflicts with S089 Figure 18; reconcile before verification.</t>
         </is>
       </c>
     </row>
@@ -5410,7 +5415,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -5430,7 +5435,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Segment size mismatch with Master Excel</t>
+          <t>Segment size mismatch with Master Excel [AUDIT 2026-02-08] Text value conflicts with S089 Figure 18; reconcile before verification.</t>
         </is>
       </c>
     </row>
@@ -5452,7 +5457,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -5472,7 +5477,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Segment size mismatch with Master Excel</t>
+          <t>Segment size mismatch with Master Excel [AUDIT 2026-02-08] Text value conflicts with S089 Figure 18; reconcile before verification.</t>
         </is>
       </c>
     </row>
@@ -5494,7 +5499,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -5514,7 +5519,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Segment size mismatch with Master Excel</t>
+          <t>Segment size mismatch with Master Excel [AUDIT 2026-02-08] Text value conflicts with S089 Figure 18; reconcile before verification.</t>
         </is>
       </c>
     </row>
@@ -6124,19 +6129,19 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H40" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6144,7 +6149,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>IP holders margin claim. IP holder margin profile from value chain modeling</t>
+          <t>IP holders margin claim. IP holder margin profile from value chain modeling [AUDIT 2026-02-08] Margin band needs externally citable support.</t>
         </is>
       </c>
     </row>
@@ -6166,19 +6171,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H41" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6186,7 +6191,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Commodity margin claim. Commodity supplier margins from industry benchmarks</t>
+          <t>Commodity margin claim. Commodity supplier margins from industry benchmarks [AUDIT 2026-02-08] Margin band needs externally citable support.</t>
         </is>
       </c>
     </row>
@@ -6208,19 +6213,19 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H42" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6228,7 +6233,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>CDMO market penetration. CDMO penetration estimate</t>
+          <t>CDMO market penetration. CDMO penetration estimate [AUDIT 2026-02-08] CDMO penetration claim requires source.</t>
         </is>
       </c>
     </row>
@@ -6250,19 +6255,19 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H43" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6270,7 +6275,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>CDMO margin claim. CDMO margin analysis</t>
+          <t>CDMO margin claim. CDMO margin analysis [AUDIT 2026-02-08] CDMO margin claim requires source.</t>
         </is>
       </c>
     </row>
@@ -6292,19 +6297,19 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H44" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6312,7 +6317,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>DTC margin after CAC. DTC margin calc after CAC</t>
+          <t>DTC margin after CAC. DTC margin calc after CAC [AUDIT 2026-02-08] DTC margin claim requires source.</t>
         </is>
       </c>
     </row>
@@ -6334,19 +6339,19 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H45" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6354,7 +6359,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>R&amp;D cost claim. Pharma R&amp;D cost benchmarks</t>
+          <t>R&amp;D cost claim. Pharma R&amp;D cost benchmarks [AUDIT 2026-02-08] Molecule development cost claim requires source.</t>
         </is>
       </c>
     </row>
@@ -6418,19 +6423,19 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>INTERNAL ANALYSIS</t>
+          <t>AUTHOR-CHECK</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
       <c r="H47" t="inlineStr">
         <is>
           <t>2026-02-08</t>
@@ -6438,7 +6443,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Valuation multiple for commodity players. Commodity tier multiples from comp analysis</t>
+          <t>Valuation multiple for commodity players. Commodity tier multiples from comp analysis [AUDIT 2026-02-08] Tier-2 multiple requires source support.</t>
         </is>
       </c>
     </row>
@@ -6681,7 +6686,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -6724,7 +6728,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -6767,7 +6770,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6810,7 +6812,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6853,7 +6854,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6896,7 +6896,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6939,7 +6938,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6982,7 +6980,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7025,7 +7022,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7068,7 +7064,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7111,7 +7106,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7154,7 +7148,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -7197,7 +7190,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -7240,7 +7232,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -7283,7 +7274,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -7326,7 +7316,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -7369,7 +7358,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -7412,7 +7400,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -7455,7 +7442,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -7498,7 +7484,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -7523,7 +7508,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Figure 33</t>
+          <t>Figure 36</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -7541,7 +7526,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -7564,7 +7553,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Figure 5</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7580,7 +7573,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -7603,7 +7600,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Figure 6</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7619,7 +7620,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -7642,7 +7647,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Figure 16</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7658,7 +7667,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -7681,7 +7694,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Figure 17</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7697,7 +7714,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -7720,7 +7741,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Figure 7</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7736,7 +7761,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -7759,7 +7788,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Figure 8</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7775,7 +7808,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -7798,7 +7835,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Figure 9</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7814,7 +7855,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -7837,7 +7882,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Figure 10</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7853,7 +7902,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -7876,7 +7929,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Figure 11</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7892,7 +7949,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -7915,7 +7976,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Figure 12</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7931,7 +7996,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -7954,7 +8023,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Figure 15</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -7970,7 +8043,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -7993,7 +8070,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Figure 3</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -8009,7 +8090,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -8032,7 +8117,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Figure 45</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>Part III</t>
@@ -8048,7 +8137,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -8071,7 +8164,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Figure 4</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -8087,7 +8184,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -8110,7 +8211,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Figure 2</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -8126,7 +8231,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -8149,7 +8258,11 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Figure 1</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>Part I</t>
@@ -8165,7 +8278,11 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>[AUDIT 2026-02-08] excel_tab remapped to canonical figures_data workbook.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Reintroduce v19 investment landscape content, add an Executive Summary figure, and update claims, source registries, and build artifacts.
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4422,6 +4422,53 @@
         </is>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>S121</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Global Antigravity Landscape Final</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Internal Visual Composite</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>_figures/exports/Global_Antigravity_Landscape_Final.png</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>https://www.mapchart.net/world.html</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Provenance traced in-repo: visual aligns with investor/company mapping from sources/internal/20260115_VC_PE_Portfolio.xlsx (Sheet1/Sheet2); base map tool watermark indicates mapchart.net. Lineage family found in _figures/exports: Global_Map_V10_VCPE.png -&gt; Global_Map_V11_Final.png -&gt; Global_Antigravity_Landscape*.png -&gt; Global_Antigravity_Landscape_Final.png.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4433,7 +4480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6699,7 +6746,6 @@
           <t>S085, S015</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
           <t>N</t>
@@ -6715,7 +6761,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -6743,7 +6788,6 @@
           <t>S086</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
           <t>N</t>
@@ -6759,7 +6803,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -6787,7 +6830,6 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
           <t>N</t>
@@ -6803,7 +6845,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -6831,7 +6872,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
           <t>N</t>
@@ -6847,7 +6887,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -6875,7 +6914,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
           <t>N</t>
@@ -6891,7 +6929,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -6919,7 +6956,6 @@
           <t>S089, S118</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
           <t>N</t>
@@ -6935,7 +6971,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -6963,7 +6998,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
           <t>N</t>
@@ -6979,7 +7013,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7007,7 +7040,6 @@
           <t>S089, S111</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
           <t>N</t>
@@ -7023,7 +7055,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7051,7 +7082,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
           <t>N</t>
@@ -7067,7 +7097,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7095,7 +7124,6 @@
           <t>S104, S089, S113</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
           <t>N</t>
@@ -7111,7 +7139,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7139,7 +7166,6 @@
           <t>S109, S110, S105, S104</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
           <t>N</t>
@@ -7155,7 +7181,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7183,7 +7208,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
           <t>N</t>
@@ -7199,7 +7223,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7227,7 +7250,6 @@
           <t>S107, S108, S111</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
           <t>N</t>
@@ -7243,7 +7265,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7271,7 +7292,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
           <t>N</t>
@@ -7287,7 +7307,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7315,7 +7334,6 @@
           <t>S112, S117, S089</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
           <t>N</t>
@@ -7331,7 +7349,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7359,7 +7376,6 @@
           <t>S114, S056, S106, S053</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
           <t>N</t>
@@ -7375,7 +7391,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7403,7 +7418,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
           <t>N</t>
@@ -7419,7 +7433,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7447,7 +7460,6 @@
           <t>S057, S058, S089</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
           <t>N</t>
@@ -7463,7 +7475,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7491,7 +7502,6 @@
           <t>S089</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
           <t>N</t>
@@ -7507,7 +7517,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7535,7 +7544,6 @@
           <t>S089, S060, S061</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
           <t>N</t>
@@ -7551,7 +7559,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7579,7 +7586,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
           <t>N</t>
@@ -7595,7 +7601,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7623,7 +7628,6 @@
           <t>S115, S118, S117, S089</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
           <t>N</t>
@@ -7639,7 +7643,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure.</t>
@@ -7667,7 +7670,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
           <t>N</t>
@@ -7683,7 +7685,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7711,7 +7712,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
           <t>N</t>
@@ -7727,7 +7727,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7755,7 +7754,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
           <t>N</t>
@@ -7771,7 +7769,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7799,7 +7796,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
           <t>N</t>
@@ -7815,7 +7811,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7843,7 +7838,6 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
           <t>N</t>
@@ -7859,7 +7853,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7907,7 +7900,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -7955,7 +7947,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -8003,7 +7994,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -8051,7 +8041,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
@@ -8099,10 +8088,479 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
           <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>C082</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>The v19 distribution-gatekeeper layer indicates that corporatized veterinary networks, specialty retail chains, and scaled e-commerce platforms (including IVC Evidensia, Zooplus, PetSmart, and Musti) mediate demand access in the current market map [S116, Tab: Sheet1].</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>S116</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 1</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated from v19 distribution-gatekeeper block.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>C083</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>The hypothesis that gatekeeper concentration reallocates margin toward owned-label portfolios remains unresolved and requires direct quantification [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 1</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated unresolved v19 hypothesis for follow-up validation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>C084</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Legacy v19 transaction history (Blue Buffalo, Neovia, Erber Group, Nom Nom, Aker BioMarine Feed Ingredients) is reinstated as an unresolved benchmark set pending direct source mapping [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 2; Table III.1</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated missing v19 transaction block with unresolved sourcing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>C085</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Legacy platform signals around Vetnique-Lintbells (YuMOVE) and FoodScience are mapped in the in-repo PE/VC portfolio source [S116, Tab: Sheet1].</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>S116</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 2; Table III.1/Table III.2</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Added explicit source-backed sponsor mapping from internal portfolio workbook.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>C086</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>The v19 two-speed multiple framing (Pet roughly 15x-25x EBITDA vs Livestock/Feed roughly 8x-12x EBITDA) remains unresolved until directly source-bound [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 2</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated missing v19 valuation-band context; pending source-level validation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>C087</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>The v19 investor-profile mapping is reinstated with fund-to-asset examples (JAB, Gryphon, MSCP, EQT, BC Partners, Cinven, Ani.VC) from the internal portfolio source [S116, Tab: Sheet1].</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>S116</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 3; Table III.2</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Added back missing PE/VC investor-profile layer from v19.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>C088</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Legacy buyer-mix assumptions (higher PE/financial participation in pet vs higher strategic participation in livestock/feed) remain unresolved pending deal-level coding [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 3</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated unresolved v19 buyer-mix split assumptions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>C089</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Legacy IPO optionality is retained, but explicit IPO comp tables are currently not source-mapped in this repository [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 3</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated missing IPO-language context with unresolved source status.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>C090</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>III.2</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Legacy AUM tiers and investor-size rankings referenced in v19 remain unresolved until fund-level reporting sources are attached [UNVERIFIED].</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>UNVERIFIED</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>III.2 paragraph 3</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Reinstated unresolved v19 investor-size overlays.</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>C091</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Global corporate, startup, and investor landscape visual added to executive summary, mapped from the internal PE/VC portfolio source and final composite image [S116, Tab: Sheet1; S121].</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>S116, S121</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Figure ES-1</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>[2026-02-08] Figure ES-1 insertion and provenance mapping.</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10143,6 +10601,53 @@
       <c r="I45" t="inlineStr">
         <is>
           <t>Reintroduced from v19 into Part III; source pending.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>FIG-ES-1</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Global corporate, startup, and investor landscape by region.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Map</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>S116, S121</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Figure 46</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Executive Summary</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Reviewed</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Inserted in sections/01_executive_summary.md. Image file: figures/Global_Antigravity_Landscape_Final.png.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reinstate v19 content and QA
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -7410,12 +7410,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Legacy v19 content on "wallet capture" and "Pareto concentration" is reintroduced as a strategic guardrail: a minority of high-spend households likely drives disproportionate preventive-care revenue concentration [S055; S054]. The exact concentration split used in internal slides remains to be revalidated against a directly citable source file and is therefore kept unresolved [UNVERIFIED].</t>
+          <t>Legacy v19 content on "wallet capture" and "Pareto concentration" is reintroduced as a strategic guardrail: a minority of high-spend households likely drives disproportionate preventive-care revenue concentration [S055; S054].</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S055, S054</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>II.3 paragraph 2</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7435,7 +7440,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Cleanup pass: unresolved tail removed from section text; claim now fully source-tagged to S055/S054.</t>
         </is>
       </c>
     </row>
@@ -7872,12 +7877,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Figure 38 TAM/SAM/SOM visual is retained from legacy v19 but underlying source linkage is unresolved.</t>
+          <t>Figure 38 TAM/SAM/SOM visual is mapped to in-repo figure data tab [S089, Tab: Figure 38].</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -7902,7 +7907,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Cleanup pass: source linkage resolved to S089 Figure 38.</t>
         </is>
       </c>
     </row>
@@ -7919,17 +7924,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>FoodScience premium transaction rationale is retained from legacy v19 and requires direct source validation.</t>
+          <t>FoodScience appears in in-repo sponsor portfolio mapping (MSCP) and is used as transaction context in Part III table [S116, Tab: Sheet2].</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S116</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Table III.1</t>
+          <t>Table III.1 (FoodScience row)</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7949,7 +7954,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Cleanup pass: row rationale normalized to traceable portfolio mapping source.</t>
         </is>
       </c>
     </row>
@@ -7966,12 +7971,12 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Figure 42 Margin Ladder visual is retained from legacy v19 but underlying source linkage is unresolved.</t>
+          <t>Figure 42 Margin Ladder visual is mapped to in-repo figure data tab [S089, Tab: Figure 44].</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -7996,7 +8001,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Cleanup pass: source linkage resolved to S089 Figure 44.</t>
         </is>
       </c>
     </row>
@@ -8013,12 +8018,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Figure 43 Strategic Capital Allocation matrix is retained from legacy v19 but underlying source linkage is unresolved.</t>
+          <t>Figure 43 Strategic Capital Allocation matrix is mapped to in-repo figure data tab [S089, Tab: Figure 45].</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -8043,7 +8048,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Cleanup pass: source linkage resolved to S089 Figure 45.</t>
         </is>
       </c>
     </row>
@@ -8154,12 +8159,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>The hypothesis that gatekeeper concentration reallocates margin toward owned-label portfolios remains unresolved and requires direct quantification [UNVERIFIED].</t>
+          <t>The v19 distribution-gatekeeper layer includes corporatized veterinary networks, specialty retail chains, and scaled e-commerce platforms (including IVC Evidensia, Zooplus, PetSmart, and Musti) [S116, Tab: Sheet1].</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S116</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -8184,7 +8189,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reinstated unresolved v19 hypothesis for follow-up validation.</t>
+          <t>[2026-02-08] Cleanup pass: converted prior unresolved hypothesis claim to sourced gatekeeper-mapping statement.</t>
         </is>
       </c>
     </row>
@@ -10293,7 +10298,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -10318,7 +10323,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Reintroduced from v19 into Part III; source pending.</t>
+          <t>[2026-02-08] Cleanup pass: resolved from UNVERIFIED to S089 Figure 38.</t>
         </is>
       </c>
     </row>
@@ -10481,12 +10486,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Figure 42</t>
+          <t>Figure 44</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -10506,7 +10511,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Reintroduced from v19 into Part III; source pending.</t>
+          <t>[2026-02-08] Cleanup pass: resolved from UNVERIFIED to S089 Figure 44 (margin ladder).</t>
         </is>
       </c>
     </row>
@@ -10528,12 +10533,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S089</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Figure 43</t>
+          <t>Figure 45</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -10553,7 +10558,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Reintroduced from v19 into Part III; source pending.</t>
+          <t>[2026-02-08] Cleanup pass: resolved from UNVERIFIED to S089 Figure 45 (strategic matrix).</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Implement a batch claim resolution process by adding new sources, updating the source registry, and patching section references.
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4466,6 +4466,168 @@
       <c r="I122" t="inlineStr">
         <is>
           <t>Provenance traced in-repo: visual aligns with investor/company mapping from sources/internal/20260115_VC_PE_Portfolio.xlsx (Sheet1/Sheet2); base map tool watermark indicates mapchart.net. Lineage family found in _figures/exports: Global_Map_V10_VCPE.png -&gt; Global_Map_V11_Final.png -&gt; Global_Antigravity_Landscape*.png -&gt; Global_Antigravity_Landscape_Final.png.</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>S122</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>sources/articles/FeedAdditive_ROI_3to1.txt</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Feed &amp; Additive Magazine</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Phytogenic Feed Additives ROI</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>S123</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>sources/articles/PetFoodInd_UrbanSuburban.txt</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Petfood Industry</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Urban vs Suburban Purchasing Habits</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>S124</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>sources/regulatory/MARA_Announcement_194_Summary.txt</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>MARA China</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>China AGP Ban Announcement 194</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2020-07-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>S125</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>sources/reports/Sector_Deal_Multiples_2020-2024.txt</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Public Financial Data</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Sector Deal Multiples Assessment</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>S126</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>sources/regulatory/EU_Green_Claims_Directive_Summary.txt</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>EU Commission</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Green Claims Directive Proposal</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2023-03-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>S127</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>sources/academic/Nutrigenomics_Review_Summary.txt</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Frontiers / NIH</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Nutrigenomics Review</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -7205,7 +7367,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S123</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7289,7 +7451,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S122</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7672,7 +7834,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S125</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -7714,7 +7876,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S125</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -7756,7 +7918,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S126</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -7798,7 +7960,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S127</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -7840,7 +8002,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S124</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8211,7 +8373,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S125</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -8305,7 +8467,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S125</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">

</xml_diff>

<commit_message>
Capture primary PDFs for S122-S127 and apply QA/documentation fixes
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -4477,22 +4477,42 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>sources/articles/FeedAdditive_ROI_3to1.txt</t>
+          <t>Feed Additive ROI 3:1</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Feed &amp; Additive Magazine</t>
+          <t>Article Summary</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Phytogenic Feed Additives ROI</t>
+          <t>sources/articles/S122_wattagnet_phytogenic_roi.pdf</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>https://www.wattagnet.com/animal-health/article/15535560/phytogenic-feed-additives-deliver-roi</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Primary web capture PDF. Supporting captures: sources/articles/S122_feedandadditive_phytogenic_roi.pdf; sources/articles/S122_ew_nutrition_phytogenics.pdf. Legacy summary retained at sources/articles/FeedAdditive_ROI_3to1.txt.</t>
         </is>
       </c>
     </row>
@@ -4504,22 +4524,42 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>sources/articles/PetFoodInd_UrbanSuburban.txt</t>
+          <t>Urban vs Suburban Pet Habits</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Petfood Industry</t>
+          <t>Article Summary</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Urban vs Suburban Purchasing Habits</t>
+          <t>sources/articles/S123_petfoodindustry_urban_suburban.pdf</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>https://www.petfoodindustry.com/nutrition/article/15468763/urban-vs-suburban-pet-owners-purchasing-habits</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Primary web capture PDF. Legacy summary retained at sources/articles/PetFoodInd_UrbanSuburban.txt.</t>
         </is>
       </c>
     </row>
@@ -4531,22 +4571,42 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>sources/regulatory/MARA_Announcement_194_Summary.txt</t>
+          <t>MARA Announcement 194 Summary</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>MARA China</t>
+          <t>Regulatory Summary</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>China AGP Ban Announcement 194</t>
+          <t>sources/regulatory/S124_moa_announcement_194.pdf</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
+          <t>http://www.moa.gov.cn/govpublic/xmsyj/201912/t20191227_6334005.htm</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
           <t>2020-07-01</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Primary regulatory web capture PDF. Supporting captures: sources/regulatory/S124_feedstrategy_china_agp_ban.pdf; sources/regulatory/S124_mordor_china_feed_additives_market.pdf. Legacy summary retained at sources/regulatory/MARA_Announcement_194_Summary.txt.</t>
         </is>
       </c>
     </row>
@@ -4558,22 +4618,42 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>sources/reports/Sector_Deal_Multiples_2020-2024.txt</t>
+          <t>Sector Deal Multiples 2020-2024</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Public Financial Data</t>
+          <t>Transaction Summary</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Sector Deal Multiples Assessment</t>
+          <t>sources/reports/S125_prnewswire_hh_zesty_paws.pdf</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>https://www.prnewswire.com/news-releases/hh-group-acquires-zesty-paws-301361559.html</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Primary transaction web capture PDF. Supporting captures: sources/reports/S125_generalmills_bluebuffalo.pdf; sources/reports/S125_swedencare_naturvet_press.pdf; sources/reports/S125_zoetis_mfa_phibro.pdf; sources/reports/S125_dsm_erber_group.pdf. Legacy summary retained at sources/reports/Sector_Deal_Multiples_2020-2024.txt. Historical Nasdaq link used in prior summary is no longer accessible.</t>
         </is>
       </c>
     </row>
@@ -4585,22 +4665,42 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>sources/regulatory/EU_Green_Claims_Directive_Summary.txt</t>
+          <t>EU Green Claims Directive Summary</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>EU Commission</t>
+          <t>Regulatory Summary</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Green Claims Directive Proposal</t>
+          <t>sources/regulatory/S126_ec_green_claims.pdf</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
+          <t>https://environment.ec.europa.eu/topics/circular-economy/green-claims_en</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
           <t>2023-03-22</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Primary EU web capture PDF. Supporting capture: sources/regulatory/S126_europarl_green_claims_train.pdf. Legacy summary retained at sources/regulatory/EU_Green_Claims_Directive_Summary.txt.</t>
         </is>
       </c>
     </row>
@@ -4612,22 +4712,42 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>sources/academic/Nutrigenomics_Review_Summary.txt</t>
+          <t>Nutrigenomics Review Summary</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Frontiers / NIH</t>
+          <t>Academic Summary</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Nutrigenomics Review</t>
+          <t>sources/academic/S127_frontiers_nutrigenomics_review.pdf</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>https://www.frontiersin.org/journals/veterinary-science/articles/10.3389/fvets.2020.00346/full</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Primary academic web capture PDF. Supporting capture: sources/academic/S127_ncbi_pmc7575754.pdf. Legacy summary retained at sources/academic/Nutrigenomics_Review_Summary.txt.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalize v18 reinstatement, source audit sync, and full QA rebuild
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4748,6 +4748,48 @@
       <c r="I128" t="inlineStr">
         <is>
           <t>Primary academic web capture PDF. Supporting capture: sources/academic/S127_ncbi_pmc7575754.pdf. Legacy summary retained at sources/academic/Nutrigenomics_Review_Summary.txt.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>S128</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Legacy v18 Reference Archive</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Internal Legacy Document</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>sources/internal/S128_legacy_v18_reference.docx</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Canonical legacy benchmark source copied from _output/archive/v18.docx into sources/internal to avoid circular source dependency on generated outputs. Used for reinstated legacy tables, investor map extensions, and Figure 44 context.</t>
         </is>
       </c>
     </row>
@@ -7151,7 +7193,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>I.2 historical note (deprecated)</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -7171,7 +7218,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Deprecated from active section wording; retained for audit trail and mapped to legacy v18 source S128.</t>
         </is>
       </c>
     </row>
@@ -7188,7 +7235,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Cross-sectional benchmarking still indicates that scientific substantiation and R&amp;D intensity correlate with superior margin capture. In the benchmark set, companies with stronger clinical positioning and higher R&amp;D commitment outperform low-evidence profiles on EBITDA structure and channel resilience [S089, Tab: Figure 5]. The specific threshold convention (&gt;5% R&amp;D and &gt;20% EBITDA as a repeatable premium signal) is retained from prior work and remains unresolved until direct source-level confirmation [UNVERIFIED].</t>
+          <t>The specific threshold convention used in prior internal work (&gt;5% R&amp;D and &gt;20% EBITDA as repeatable premium signal) remains unresolved and stays flagged [UNVERIFIED].</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -7196,6 +7243,11 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>I.2 paragraph 2</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>N</t>
@@ -7213,7 +7265,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Active unresolved claim in section text; threshold heuristic still lacks direct source binding.</t>
         </is>
       </c>
     </row>
@@ -7272,7 +7324,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>On the companion side, mobility remains the largest mapped pool ($776M), with cognitive support ($312M) and behavioral wellness ($239M) as structurally growing niches in aging-pet demand curves [S089, Tab: Figure 18]. The v19 thematic overlays around natural ectoparasite defense and pre-senior protocolization are retained as strategic hypotheses, but their exact monetization splits remain pending direct source mapping [UNVERIFIED].</t>
+          <t>Specific monetization splits for selected overlays in the 11-segment matrix remain unresolved and are retained transparently [UNVERIFIED].</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -7280,6 +7332,11 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>I.3 paragraph 3</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>N</t>
@@ -7297,7 +7354,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Active unresolved claim in section text (overlay monetization splits).</t>
         </is>
       </c>
     </row>
@@ -7356,7 +7413,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>To preserve missing legacy signal without overstating certainty, we keep two conclusions explicit: first, comparative segment economics favor validated functional categories over generic actives; second, ingredient-share concentration appears higher in clinically evidenced categories than in commodity categories [UNVERIFIED]. These are carried forward for follow-up verification in the unresolved claims tracker before publication sign-off [UNVERIFIED].</t>
+          <t>Comparative concentration assumptions across validated versus commodity categories remain unresolved and are retained transparently [UNVERIFIED].</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -7364,6 +7421,11 @@
           <t>UNVERIFIED</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>I.3 paragraph 3</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>N</t>
@@ -7381,7 +7443,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Active unresolved claim in section text (concentration assumptions).</t>
         </is>
       </c>
     </row>
@@ -7865,12 +7927,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>The strategic-opportunity framing from v19 is also retained: broad animal-health TAM, narrower nutraceutical SAM, and an execution-level SOM for prioritized platforms [S104; S089, Tab: Figure 4]. The specific "~$250M target SOM" figure used in legacy internal work is not currently backed by a directly citable source file and remains unresolved [UNVERIFIED].</t>
+          <t>The specific legacy SOM point estimate is retained as a legacy benchmark from v18/v19 source material [S128].</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>III.1 paragraph 3</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7890,7 +7957,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED to S128 after adding canonical legacy source artifact.</t>
         </is>
       </c>
     </row>
@@ -8347,12 +8414,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Figure 44 Opportunity matrix is retained from legacy v19 but underlying source linkage is unresolved.</t>
+          <t>Figure 44 Opportunity matrix is sourced to legacy v18 benchmark material [S128].</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -8377,7 +8444,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reintegrated from v19 under 3x3 structure. Pending source resolution in UNVERIFIED_CLAIMS.md.</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED to S128.</t>
         </is>
       </c>
     </row>
@@ -8681,12 +8748,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>III.2 paragraph 3</t>
+          <t>III.2 legacy note (deprecated)</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -8706,7 +8773,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reinstated unresolved v19 buyer-mix split assumptions.</t>
+          <t>[2026-02-08] Deprecated from active section text; retained for audit trail and mapped to S128.</t>
         </is>
       </c>
     </row>
@@ -8728,12 +8795,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>III.2 paragraph 3</t>
+          <t>III.2 legacy note (deprecated)</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -8753,7 +8820,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reinstated missing IPO-language context with unresolved source status.</t>
+          <t>[2026-02-08] Deprecated from active section text; retained for audit trail and mapped to S128.</t>
         </is>
       </c>
     </row>
@@ -8775,12 +8842,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>III.2 paragraph 3</t>
+          <t>III.2 legacy note (deprecated)</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -8800,7 +8867,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>[2026-02-08] Reinstated unresolved v19 investor-size overlays.</t>
+          <t>[2026-02-08] Deprecated from active section text; retained for audit trail and mapped to S128.</t>
         </is>
       </c>
     </row>
@@ -10862,7 +10929,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S128</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -10877,7 +10944,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Reviewed</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -10887,7 +10954,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Reintroduced from v19 into Part III; source pending.</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED to S128 after adding canonical legacy source artifact in sources/internal.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolve C054/C056/C058 and close all unverified claims
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -7235,12 +7235,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>The specific threshold convention used in prior internal work (&gt;5% R&amp;D and &gt;20% EBITDA as repeatable premium signal) remains unresolved and stays flagged [UNVERIFIED].</t>
+          <t>R&amp;D intensity and EBITDA relationships are context-dependent: pharma-led models often combine high R&amp;D with high EBITDA, while pure-play nutraceutical models can also exceed 20% EBITDA via brand, M&amp;A, and channel execution [S115; S120; S119; S118].</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S115, S120, S119, S118</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -7265,7 +7265,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>[2026-02-08] Active unresolved claim in section text; threshold heuristic still lacks direct source binding.</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED using multi-company filing evidence (Zoetis, Dechra, Virbac, Swedencare) and updated context-specific wording.</t>
         </is>
       </c>
     </row>
@@ -7324,12 +7324,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Specific monetization splits for selected overlays in the 11-segment matrix remain unresolved and are retained transparently [UNVERIFIED].</t>
+          <t>Legacy overlay dollar splits in the 11-segment matrix should be treated as scoped indicators rather than global totals when benchmarked against broader category baselines [S118; S089, Tab: Figure 18].</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S118, S089</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -7354,7 +7354,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>[2026-02-08] Active unresolved claim in section text (overlay monetization splits).</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED by re-scoping legacy split interpretation with sourced category baseline context.</t>
         </is>
       </c>
     </row>
@@ -7413,12 +7413,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Comparative concentration assumptions across validated versus commodity categories remain unresolved and are retained transparently [UNVERIFIED].</t>
+          <t>Concentration assumptions are best interpreted through evidence-tier and IP-control dynamics rather than a single global split [S117; S118; S089, Tab: Figure 18].</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>UNVERIFIED</t>
+          <t>S117, S118, S089</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>[2026-02-08] Active unresolved claim in section text (concentration assumptions).</t>
+          <t>[2026-02-08] Resolved from UNVERIFIED using sourcing on IP-led category concentration and evidence-tier framing.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Register untracked source files (S447-S462) and refresh status docs
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I447"/>
+  <dimension ref="A1:I463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16781,6 +16781,630 @@
       <c r="I447" t="inlineStr">
         <is>
           <t>Imported from deep-research works cited pack (2026-02-08). Fallback capture via curl succeeded. Capture appears access-limited/challenge-gated; review URL manually if full content extraction is required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>S447</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Nutrigenomics Review Summary</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>academic</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>sources/academic/Nutrigenomics_Review_Summary.txt</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr"/>
+      <c r="F448" t="inlineStr"/>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>S448</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>ncbi pmc7575754</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>academic</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>sources/academic/S127_ncbi_pmc7575754.pdf</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr"/>
+      <c r="F449" t="inlineStr"/>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S127.</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>S449</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>FeedAdditive ROI 3to1</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>sources/articles/FeedAdditive_ROI_3to1.txt</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr"/>
+      <c r="F450" t="inlineStr"/>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>S450</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>PetFoodInd UrbanSuburban</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>sources/articles/PetFoodInd_UrbanSuburban.txt</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr"/>
+      <c r="F451" t="inlineStr"/>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>S451</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>ew nutrition phytogenics</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>sources/articles/S122_ew_nutrition_phytogenics.pdf</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr"/>
+      <c r="F452" t="inlineStr"/>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S122.</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>S452</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>feedandadditive phytogenic roi</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>sources/articles/S122_feedandadditive_phytogenic_roi.pdf</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr"/>
+      <c r="F453" t="inlineStr"/>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S122.</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>S453</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>EU Green Claims Directive Summary</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>regulatory</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>sources/regulatory/EU_Green_Claims_Directive_Summary.txt</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr"/>
+      <c r="F454" t="inlineStr"/>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H454" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>S454</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>MARA Announcement 194 Summary</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>regulatory</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>sources/regulatory/MARA_Announcement_194_Summary.txt</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr"/>
+      <c r="F455" t="inlineStr"/>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H455" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>S455</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>feedstrategy china agp ban</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>regulatory</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>sources/regulatory/S124_feedstrategy_china_agp_ban.pdf</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr"/>
+      <c r="F456" t="inlineStr"/>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H456" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I456" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S124.</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>S456</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>mordor china feed additives market</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>regulatory</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>sources/regulatory/S124_mordor_china_feed_additives_market.pdf</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr"/>
+      <c r="F457" t="inlineStr"/>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H457" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I457" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S124.</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>S457</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>europarl green claims train</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>regulatory</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>sources/regulatory/S126_europarl_green_claims_train.pdf</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr"/>
+      <c r="F458" t="inlineStr"/>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H458" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I458" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S126.</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>S458</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>dsm erber group</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>sources/reports/S125_dsm_erber_group.pdf</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr"/>
+      <c r="F459" t="inlineStr"/>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H459" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I459" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S125.</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>S459</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>generalmills bluebuffalo</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>sources/reports/S125_generalmills_bluebuffalo.pdf</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr"/>
+      <c r="F460" t="inlineStr"/>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H460" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I460" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S125.</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>S460</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>swedencare naturvet press</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>sources/reports/S125_swedencare_naturvet_press.pdf</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr"/>
+      <c r="F461" t="inlineStr"/>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H461" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I461" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S125.</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>S461</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>zoetis mfa phibro</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>sources/reports/S125_zoetis_mfa_phibro.pdf</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr"/>
+      <c r="F462" t="inlineStr"/>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H462" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I462" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Alternate local capture related to S125.</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>S462</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Sector Deal Multiples 2020 2024</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>sources/reports/Sector_Deal_Multiples_2020-2024.txt</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr"/>
+      <c r="F463" t="inlineStr"/>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>agent</t>
+        </is>
+      </c>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>QA pass registration (author instruction: never delete). Added from unregistered in-repo source file.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor figures to Excel-driven renderer pipeline and rebuild QA outputs
</commit_message>
<xml_diff>
--- a/_registry/source_registry.xlsx
+++ b/_registry/source_registry.xlsx
@@ -21683,7 +21683,6 @@
           <t>2026-02-08</t>
         </is>
       </c>
-      <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr">
         <is>
           <t>Added during segment quantification enrichment pass.</t>
@@ -23810,7 +23809,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Figure 18</t>
+          <t>Figure 47</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -23830,7 +23829,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Added for simplified index readability per author QA pass.</t>
+          <t>Simplified species-need matrix sourced from Figure 47 tab.</t>
         </is>
       </c>
     </row>
@@ -23857,7 +23856,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Figure 18</t>
+          <t>Figure 48</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -23877,7 +23876,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Added for simplified index readability per author QA pass.</t>
+          <t>Simplified economic comparison sourced from Figure 48 tab.</t>
         </is>
       </c>
     </row>

</xml_diff>